<commit_message>
diamonds is_deleted from excel sheet
</commit_message>
<xml_diff>
--- a/public/admin_assets/sample/Polish-Diamonds.xlsx
+++ b/public/admin_assets/sample/Polish-Diamonds.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Xampp\htdocs\janvilgd\public\admin_assets\sample\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="1965" windowWidth="24240" windowHeight="13500"/>
+    <workbookView xWindow="1272" yWindow="1968" windowWidth="24240" windowHeight="13500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -52,9 +57,6 @@
     <t>Video Link</t>
   </si>
   <si>
-    <t>Cut Grade</t>
-  </si>
-  <si>
     <t>Polish</t>
   </si>
   <si>
@@ -106,20 +108,23 @@
     <t>image-1</t>
   </si>
   <si>
-    <t>image-2</t>
-  </si>
-  <si>
-    <t>image-3</t>
-  </si>
-  <si>
-    <t>image-4</t>
+    <t>Cut</t>
+  </si>
+  <si>
+    <t>COMMENT</t>
+  </si>
+  <si>
+    <t>LOCATION</t>
+  </si>
+  <si>
+    <t>is_deleted</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -128,25 +133,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -157,7 +146,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -167,37 +156,45 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -502,7 +499,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -510,18 +507,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:AC1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="36.75" customWidth="1"/>
+    <col min="8" max="8" width="36.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -547,72 +542,68 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AC1" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="G2" s="3"/>
-      <c r="H2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>